<commit_message>
remove last 3 columns in second tab
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3094" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3093" uniqueCount="100">
   <si>
     <t>Waterpeil aanpassingen IJzer</t>
   </si>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>4 x 1,5m</t>
-  </si>
-  <si>
-    <t>3,00m TAW I.o. van TL in verband met werken peilmeter. Aanhouden tot 18/04 12u</t>
   </si>
   <si>
     <t>yzerstar</t>
@@ -10373,10 +10370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q303"/>
+  <dimension ref="A1:P303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14623,7 +14620,7 @@
       <c r="M144" s="52"/>
       <c r="N144" s="53"/>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A145" s="41"/>
       <c r="B145" s="42">
         <v>0.47916666666666669</v>
@@ -14652,11 +14649,8 @@
       <c r="N145" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="Q145" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A146" s="41"/>
       <c r="B146" s="42">
         <v>0.625</v>
@@ -14684,7 +14678,7 @@
       </c>
       <c r="N146" s="54"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" s="41"/>
       <c r="B147" s="42">
         <v>0.72916666666666663</v>
@@ -14707,10 +14701,10 @@
         <v>33</v>
       </c>
       <c r="N147" s="54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A148" s="41"/>
       <c r="B148" s="42">
         <v>0.75</v>
@@ -14750,7 +14744,7 @@
       </c>
       <c r="N148" s="54"/>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A149" s="41"/>
       <c r="B149" s="42">
         <v>0.79166666666666663</v>
@@ -14774,7 +14768,7 @@
       <c r="M149" s="52"/>
       <c r="N149" s="54"/>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A150" s="41"/>
       <c r="B150" s="42">
         <v>0.80902777777777779</v>
@@ -14802,7 +14796,7 @@
       </c>
       <c r="N150" s="54"/>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A151" s="41"/>
       <c r="B151" s="42">
         <v>0.86458333333333337</v>
@@ -14832,7 +14826,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A152" s="41">
         <v>45400</v>
       </c>
@@ -14864,7 +14858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A153" s="41"/>
       <c r="B153" s="42">
         <v>0.22916666666666666</v>
@@ -14892,7 +14886,7 @@
       </c>
       <c r="N153" s="54"/>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A154" s="41"/>
       <c r="B154" s="42">
         <v>0.33333333333333331</v>
@@ -14928,7 +14922,7 @@
       <c r="M154" s="52"/>
       <c r="N154" s="54"/>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A155" s="41"/>
       <c r="B155" s="42">
         <v>0.34722222222222227</v>
@@ -14958,7 +14952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A156" s="41"/>
       <c r="B156" s="42">
         <v>0.53819444444444442</v>
@@ -14988,7 +14982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A157" s="41"/>
       <c r="B157" s="42">
         <v>0.65277777777777779</v>
@@ -15016,7 +15010,7 @@
       </c>
       <c r="N157" s="54"/>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A158" s="41"/>
       <c r="B158" s="42">
         <v>0.75</v>
@@ -15050,7 +15044,7 @@
       <c r="M158" s="52"/>
       <c r="N158" s="54"/>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A159" s="41"/>
       <c r="B159" s="42">
         <v>0.79166666666666663</v>
@@ -15074,7 +15068,7 @@
       <c r="M159" s="52"/>
       <c r="N159" s="54"/>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A160" s="41"/>
       <c r="B160" s="42">
         <v>0.88888888888888884</v>

</xml_diff>

<commit_message>
23 april 2023 to 2024
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
@@ -10372,8 +10372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="G187" sqref="G187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16292,7 +16292,7 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A201" s="41">
-        <v>45040</v>
+        <v>45406</v>
       </c>
       <c r="B201" s="42">
         <v>1.3888888888888888E-2</v>
@@ -18976,8 +18976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P323"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
toevoegen 'einde omgekeerd spuibeheer' op 29 april 7h40
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_Ijzer_2024.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3093" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3094" uniqueCount="100">
   <si>
     <t>Waterpeil aanpassingen IJzer</t>
   </si>
@@ -1442,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P325"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="K145" sqref="K145"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="J131" sqref="A131:XFD131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10372,8 +10372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="G187" sqref="G187"/>
+    <sheetView tabSelected="1" topLeftCell="J235" workbookViewId="0">
+      <selection activeCell="N245" sqref="N245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17630,7 +17630,9 @@
       <c r="M245" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="N245" s="54"/>
+      <c r="N245" s="54" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A246" s="41"/>
@@ -18977,7 +18979,7 @@
   <dimension ref="A1:P323"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="J16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>